<commit_message>
Started removing invalid news articles from dataset
</commit_message>
<xml_diff>
--- a/data/local_news_articles.xlsx
+++ b/data/local_news_articles.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\ics5110-news-analysis\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\ics5110-news-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4AD54C55-4DBB-477F-8CDE-123099A35B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B0470B-1D1B-40C6-AC13-5FAC0A5C573B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D9D61695-E2F4-4809-8028-5BCD779FF01A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D9D61695-E2F4-4809-8028-5BCD779FF01A}"/>
   </bookViews>
   <sheets>
     <sheet name="local_news_articles" sheetId="1" r:id="rId1"/>
@@ -8295,31 +8295,31 @@
   <dimension ref="A1:N322"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G70" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H146" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I71" sqref="I71"/>
+      <selection pane="bottomRight" activeCell="I162" sqref="I162"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="110.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="110.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="84.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="148.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="182.140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="118.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="211.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="65.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="84.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="148.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="182.109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="118.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="211.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="65.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8363,7 +8363,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>40</v>
       </c>
@@ -8407,7 +8407,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="225" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>42</v>
       </c>
@@ -8451,7 +8451,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="165" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="144" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>46</v>
       </c>
@@ -8495,7 +8495,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>53</v>
       </c>
@@ -8539,7 +8539,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="210" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>79</v>
       </c>
@@ -8583,7 +8583,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="180" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>86</v>
       </c>
@@ -8627,7 +8627,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>287</v>
       </c>
@@ -8671,7 +8671,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>313</v>
       </c>
@@ -8715,7 +8715,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="165" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>317</v>
       </c>
@@ -8759,7 +8759,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>361</v>
       </c>
@@ -8803,7 +8803,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>370</v>
       </c>
@@ -8847,7 +8847,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>381</v>
       </c>
@@ -8891,7 +8891,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>404</v>
       </c>
@@ -8935,7 +8935,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>405</v>
       </c>
@@ -8979,7 +8979,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>407</v>
       </c>
@@ -9023,7 +9023,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>408</v>
       </c>
@@ -9067,7 +9067,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>416</v>
       </c>
@@ -9111,7 +9111,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>522</v>
       </c>
@@ -9155,7 +9155,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>607</v>
       </c>
@@ -9199,7 +9199,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>640</v>
       </c>
@@ -9243,7 +9243,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="345" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>645</v>
       </c>
@@ -9287,7 +9287,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="150" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>654</v>
       </c>
@@ -9331,7 +9331,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>679</v>
       </c>
@@ -9375,7 +9375,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>685</v>
       </c>
@@ -9419,7 +9419,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>692</v>
       </c>
@@ -9463,7 +9463,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>695</v>
       </c>
@@ -9507,7 +9507,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>751</v>
       </c>
@@ -9551,7 +9551,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>760</v>
       </c>
@@ -9595,7 +9595,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="300" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>894</v>
       </c>
@@ -9639,7 +9639,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>933</v>
       </c>
@@ -9683,7 +9683,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>941</v>
       </c>
@@ -9727,7 +9727,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>964</v>
       </c>
@@ -9771,7 +9771,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>974</v>
       </c>
@@ -9815,7 +9815,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1015</v>
       </c>
@@ -9859,7 +9859,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>1034</v>
       </c>
@@ -9903,7 +9903,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1059</v>
       </c>
@@ -9947,7 +9947,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1165</v>
       </c>
@@ -9991,7 +9991,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1227</v>
       </c>
@@ -10035,7 +10035,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="150" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>1245</v>
       </c>
@@ -10079,7 +10079,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="180" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>1274</v>
       </c>
@@ -10123,7 +10123,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>1275</v>
       </c>
@@ -10167,7 +10167,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>1286</v>
       </c>
@@ -10211,7 +10211,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="345" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="288" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>1352</v>
       </c>
@@ -10255,7 +10255,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>1380</v>
       </c>
@@ -10299,7 +10299,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="165" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" ht="144" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>1387</v>
       </c>
@@ -10343,7 +10343,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>1388</v>
       </c>
@@ -10387,7 +10387,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>1467</v>
       </c>
@@ -10431,7 +10431,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>1489</v>
       </c>
@@ -10475,7 +10475,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>1490</v>
       </c>
@@ -10519,7 +10519,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>1509</v>
       </c>
@@ -10563,7 +10563,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>1718</v>
       </c>
@@ -10607,7 +10607,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>1745</v>
       </c>
@@ -10651,7 +10651,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>1769</v>
       </c>
@@ -10695,7 +10695,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>1776</v>
       </c>
@@ -10739,7 +10739,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>1808</v>
       </c>
@@ -10783,7 +10783,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="150" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>1814</v>
       </c>
@@ -10827,7 +10827,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>1822</v>
       </c>
@@ -10871,7 +10871,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>1856</v>
       </c>
@@ -10915,7 +10915,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>1860</v>
       </c>
@@ -10959,7 +10959,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>1882</v>
       </c>
@@ -11003,7 +11003,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>1967</v>
       </c>
@@ -11047,7 +11047,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>1989</v>
       </c>
@@ -11091,7 +11091,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="285" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>2022</v>
       </c>
@@ -11135,7 +11135,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>2028</v>
       </c>
@@ -11179,7 +11179,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="255" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>2040</v>
       </c>
@@ -11223,7 +11223,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>2080</v>
       </c>
@@ -11267,7 +11267,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="360" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>2087</v>
       </c>
@@ -11311,7 +11311,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="165" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" ht="144" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>2092</v>
       </c>
@@ -11355,7 +11355,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>2101</v>
       </c>
@@ -11399,7 +11399,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="180" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" ht="144" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>2137</v>
       </c>
@@ -11443,7 +11443,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>2157</v>
       </c>
@@ -11487,7 +11487,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>2201</v>
       </c>
@@ -11531,7 +11531,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>2259</v>
       </c>
@@ -11575,7 +11575,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="285" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>2271</v>
       </c>
@@ -11619,7 +11619,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>2275</v>
       </c>
@@ -11663,7 +11663,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="405" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>2285</v>
       </c>
@@ -11707,7 +11707,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>2301</v>
       </c>
@@ -11751,7 +11751,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>2409</v>
       </c>
@@ -11795,7 +11795,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>2419</v>
       </c>
@@ -11839,7 +11839,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="165" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" ht="144" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>2452</v>
       </c>
@@ -11883,7 +11883,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>2461</v>
       </c>
@@ -11927,7 +11927,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>2492</v>
       </c>
@@ -11971,7 +11971,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>2557</v>
       </c>
@@ -12015,7 +12015,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>2658</v>
       </c>
@@ -12059,7 +12059,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>2666</v>
       </c>
@@ -12103,7 +12103,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="150" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>2745</v>
       </c>
@@ -12147,7 +12147,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>2792</v>
       </c>
@@ -12191,7 +12191,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="89" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>2849</v>
       </c>
@@ -12235,7 +12235,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>2853</v>
       </c>
@@ -12279,7 +12279,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>2864</v>
       </c>
@@ -12323,7 +12323,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>2872</v>
       </c>
@@ -12367,7 +12367,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>2873</v>
       </c>
@@ -12411,7 +12411,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="255" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" ht="216" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>2927</v>
       </c>
@@ -12455,7 +12455,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>2940</v>
       </c>
@@ -12499,7 +12499,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>2959</v>
       </c>
@@ -12543,7 +12543,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>2974</v>
       </c>
@@ -12587,7 +12587,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="210" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>2975</v>
       </c>
@@ -12631,7 +12631,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>3001</v>
       </c>
@@ -12675,7 +12675,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>3009</v>
       </c>
@@ -12719,7 +12719,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>3076</v>
       </c>
@@ -12763,7 +12763,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="102" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>3090</v>
       </c>
@@ -12807,7 +12807,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>3095</v>
       </c>
@@ -12851,7 +12851,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="104" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>3100</v>
       </c>
@@ -12895,7 +12895,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>3139</v>
       </c>
@@ -12939,7 +12939,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="106" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>3169</v>
       </c>
@@ -12983,7 +12983,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>3197</v>
       </c>
@@ -13027,7 +13027,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>3204</v>
       </c>
@@ -13071,7 +13071,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>3206</v>
       </c>
@@ -13115,7 +13115,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>3218</v>
       </c>
@@ -13159,7 +13159,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="195" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>3220</v>
       </c>
@@ -13203,7 +13203,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="112" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>3255</v>
       </c>
@@ -13247,7 +13247,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>3315</v>
       </c>
@@ -13291,7 +13291,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="114" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>3408</v>
       </c>
@@ -13335,7 +13335,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="115" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>3410</v>
       </c>
@@ -13379,7 +13379,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="116" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>3423</v>
       </c>
@@ -13423,7 +13423,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="117" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>3442</v>
       </c>
@@ -13467,7 +13467,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="118" spans="1:14" ht="210" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:14" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>3443</v>
       </c>
@@ -13511,7 +13511,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>3456</v>
       </c>
@@ -13555,7 +13555,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="225" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:14" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>3478</v>
       </c>
@@ -13599,7 +13599,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="121" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>3497</v>
       </c>
@@ -13643,7 +13643,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="122" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>3535</v>
       </c>
@@ -13687,7 +13687,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="123" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>3551</v>
       </c>
@@ -13731,7 +13731,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="124" spans="1:14" ht="195" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:14" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>3558</v>
       </c>
@@ -13775,7 +13775,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="125" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>3563</v>
       </c>
@@ -13819,7 +13819,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="126" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>3586</v>
       </c>
@@ -13863,7 +13863,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="127" spans="1:14" ht="375" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:14" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>3588</v>
       </c>
@@ -13907,7 +13907,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="128" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>3601</v>
       </c>
@@ -13951,7 +13951,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="129" spans="1:14" ht="195" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:14" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>3604</v>
       </c>
@@ -13995,7 +13995,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="130" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>3615</v>
       </c>
@@ -14039,7 +14039,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="131" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>3626</v>
       </c>
@@ -14083,7 +14083,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="132" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>3635</v>
       </c>
@@ -14127,7 +14127,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="133" spans="1:14" ht="240" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:14" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>3653</v>
       </c>
@@ -14171,7 +14171,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="134" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>3671</v>
       </c>
@@ -14215,7 +14215,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="135" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>3699</v>
       </c>
@@ -14259,7 +14259,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="136" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>3704</v>
       </c>
@@ -14303,7 +14303,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="137" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>3740</v>
       </c>
@@ -14347,7 +14347,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="138" spans="1:14" ht="165" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:14" ht="144" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>3743</v>
       </c>
@@ -14391,7 +14391,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="139" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>3747</v>
       </c>
@@ -14435,7 +14435,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="140" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>3749</v>
       </c>
@@ -14479,7 +14479,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="141" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>3766</v>
       </c>
@@ -14523,7 +14523,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="142" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>3809</v>
       </c>
@@ -14567,7 +14567,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="143" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>3823</v>
       </c>
@@ -14611,7 +14611,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="144" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>3827</v>
       </c>
@@ -14655,7 +14655,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="145" spans="1:14" ht="240" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:14" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>3834</v>
       </c>
@@ -14699,7 +14699,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="146" spans="1:14" ht="225" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:14" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>3861</v>
       </c>
@@ -14743,7 +14743,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="147" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>3885</v>
       </c>
@@ -14787,7 +14787,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="148" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>3900</v>
       </c>
@@ -14831,7 +14831,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="149" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>3905</v>
       </c>
@@ -14875,7 +14875,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="150" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>3910</v>
       </c>
@@ -14919,7 +14919,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="151" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>3929</v>
       </c>
@@ -14963,7 +14963,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="152" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>3938</v>
       </c>
@@ -15007,7 +15007,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="153" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>3964</v>
       </c>
@@ -15051,7 +15051,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="154" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>3966</v>
       </c>
@@ -15095,7 +15095,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="155" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>3976</v>
       </c>
@@ -15139,7 +15139,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="156" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>3989</v>
       </c>
@@ -15183,7 +15183,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="157" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>3991</v>
       </c>
@@ -15227,7 +15227,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="158" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>3999</v>
       </c>
@@ -15271,7 +15271,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="159" spans="1:14" ht="180" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>4007</v>
       </c>
@@ -15315,7 +15315,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="160" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>4014</v>
       </c>
@@ -15359,7 +15359,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="161" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>4024</v>
       </c>
@@ -15403,7 +15403,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="162" spans="1:14" ht="150" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>4034</v>
       </c>
@@ -15447,7 +15447,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="163" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>4049</v>
       </c>
@@ -15491,7 +15491,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="164" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>4066</v>
       </c>
@@ -15535,7 +15535,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="165" spans="1:14" ht="255" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:14" ht="216" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>4067</v>
       </c>
@@ -15579,7 +15579,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="166" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>4087</v>
       </c>
@@ -15623,7 +15623,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="167" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>4093</v>
       </c>
@@ -15667,7 +15667,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="168" spans="1:14" ht="165" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:14" ht="144" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>4110</v>
       </c>
@@ -15711,7 +15711,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="169" spans="1:14" ht="270" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:14" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>4167</v>
       </c>
@@ -15755,7 +15755,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="170" spans="1:14" ht="150" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>4208</v>
       </c>
@@ -15799,7 +15799,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="171" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>102356</v>
       </c>
@@ -15843,7 +15843,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="172" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>113265</v>
       </c>
@@ -15887,7 +15887,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="173" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>130030</v>
       </c>
@@ -15931,7 +15931,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="174" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>136487</v>
       </c>
@@ -15975,7 +15975,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="175" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>139548</v>
       </c>
@@ -16019,7 +16019,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="176" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>141175</v>
       </c>
@@ -16063,7 +16063,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="177" spans="1:14" ht="150" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>167578</v>
       </c>
@@ -16107,7 +16107,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="178" spans="1:14" ht="270" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:14" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>178241</v>
       </c>
@@ -16151,7 +16151,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="179" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>190828</v>
       </c>
@@ -16195,7 +16195,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="180" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>220724</v>
       </c>
@@ -16239,7 +16239,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="181" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>226588</v>
       </c>
@@ -16283,7 +16283,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="182" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>227172</v>
       </c>
@@ -16327,7 +16327,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="183" spans="1:14" ht="240" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:14" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>297729</v>
       </c>
@@ -16371,7 +16371,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="184" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>297731</v>
       </c>
@@ -16415,7 +16415,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="185" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>306381</v>
       </c>
@@ -16459,7 +16459,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="186" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>353518</v>
       </c>
@@ -16503,7 +16503,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="187" spans="1:14" ht="255" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:14" ht="216" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>353524</v>
       </c>
@@ -16547,7 +16547,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="188" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>353525</v>
       </c>
@@ -16591,7 +16591,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="189" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>353565</v>
       </c>
@@ -16635,7 +16635,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="190" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>386182</v>
       </c>
@@ -16679,7 +16679,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="191" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>386207</v>
       </c>
@@ -16723,7 +16723,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="192" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>386270</v>
       </c>
@@ -16767,7 +16767,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="193" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>386315</v>
       </c>
@@ -16811,7 +16811,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="194" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>450477</v>
       </c>
@@ -16852,7 +16852,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="195" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>450529</v>
       </c>
@@ -16890,7 +16890,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="196" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>451726</v>
       </c>
@@ -16934,7 +16934,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="197" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>455412</v>
       </c>
@@ -16972,7 +16972,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="198" spans="1:14" ht="225" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:14" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>467108</v>
       </c>
@@ -17016,7 +17016,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="199" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>467110</v>
       </c>
@@ -17060,7 +17060,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="200" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>467164</v>
       </c>
@@ -17104,7 +17104,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="201" spans="1:14" ht="150" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>467167</v>
       </c>
@@ -17148,7 +17148,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="202" spans="1:14" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:14" ht="360" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>467185</v>
       </c>
@@ -17192,7 +17192,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="203" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>467297</v>
       </c>
@@ -17236,7 +17236,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="204" spans="1:14" ht="180" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>489138</v>
       </c>
@@ -17280,7 +17280,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="205" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>489339</v>
       </c>
@@ -17324,7 +17324,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="206" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>489370</v>
       </c>
@@ -17368,7 +17368,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="207" spans="1:14" ht="210" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:14" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>489424</v>
       </c>
@@ -17412,7 +17412,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="208" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>489475</v>
       </c>
@@ -17456,7 +17456,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="209" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>489580</v>
       </c>
@@ -17500,7 +17500,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="210" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>489720</v>
       </c>
@@ -17544,7 +17544,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="211" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>489728</v>
       </c>
@@ -17588,7 +17588,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="212" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>489733</v>
       </c>
@@ -17632,7 +17632,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="213" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>489878</v>
       </c>
@@ -17676,7 +17676,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="214" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>489884</v>
       </c>
@@ -17720,7 +17720,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="215" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>489889</v>
       </c>
@@ -17764,7 +17764,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="216" spans="1:14" ht="150" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>489990</v>
       </c>
@@ -17808,7 +17808,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="217" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>489993</v>
       </c>
@@ -17852,7 +17852,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="218" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>490008</v>
       </c>
@@ -17896,7 +17896,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="219" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>490010</v>
       </c>
@@ -17940,7 +17940,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="220" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>490073</v>
       </c>
@@ -17984,7 +17984,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="221" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>490101</v>
       </c>
@@ -18028,7 +18028,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="222" spans="1:14" ht="270" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:14" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>490160</v>
       </c>
@@ -18072,7 +18072,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="223" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>490165</v>
       </c>
@@ -18116,7 +18116,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="224" spans="1:14" ht="225" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:14" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>490183</v>
       </c>
@@ -18160,7 +18160,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="225" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>490206</v>
       </c>
@@ -18204,7 +18204,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="226" spans="1:14" ht="165" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:14" ht="144" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>490267</v>
       </c>
@@ -18248,7 +18248,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="227" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>490329</v>
       </c>
@@ -18292,7 +18292,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="228" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>490371</v>
       </c>
@@ -18336,7 +18336,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="229" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>490568</v>
       </c>
@@ -18380,7 +18380,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="230" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>490632</v>
       </c>
@@ -18424,7 +18424,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="231" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>490653</v>
       </c>
@@ -18468,7 +18468,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="232" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>490684</v>
       </c>
@@ -18512,7 +18512,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="233" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>490685</v>
       </c>
@@ -18556,7 +18556,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="234" spans="1:14" ht="255" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:14" ht="216" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>490697</v>
       </c>
@@ -18600,7 +18600,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="235" spans="1:14" ht="270" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:14" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>490742</v>
       </c>
@@ -18644,7 +18644,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="236" spans="1:14" ht="285" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:14" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>490746</v>
       </c>
@@ -18688,7 +18688,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="237" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>490815</v>
       </c>
@@ -18729,7 +18729,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="238" spans="1:14" ht="195" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:14" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>490929</v>
       </c>
@@ -18773,7 +18773,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="239" spans="1:14" ht="180" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>490945</v>
       </c>
@@ -18817,7 +18817,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="240" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>491011</v>
       </c>
@@ -18861,7 +18861,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="241" spans="1:14" ht="210" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:14" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>491047</v>
       </c>
@@ -18905,7 +18905,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="242" spans="1:14" ht="165" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:14" ht="144" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>491118</v>
       </c>
@@ -18949,7 +18949,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="243" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>491134</v>
       </c>
@@ -18993,7 +18993,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="244" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>491226</v>
       </c>
@@ -19037,7 +19037,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="245" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>491258</v>
       </c>
@@ -19081,7 +19081,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="246" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>491307</v>
       </c>
@@ -19125,7 +19125,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="247" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>491334</v>
       </c>
@@ -19169,7 +19169,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="248" spans="1:14" ht="150" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>491371</v>
       </c>
@@ -19213,7 +19213,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="249" spans="1:14" ht="150" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>491380</v>
       </c>
@@ -19257,7 +19257,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="250" spans="1:14" ht="225" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:14" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>491437</v>
       </c>
@@ -19301,7 +19301,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="251" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>491489</v>
       </c>
@@ -19345,7 +19345,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="252" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>491557</v>
       </c>
@@ -19389,7 +19389,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="253" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>491568</v>
       </c>
@@ -19433,7 +19433,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="254" spans="1:14" ht="165" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:14" ht="144" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>491640</v>
       </c>
@@ -19477,7 +19477,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="255" spans="1:14" ht="195" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>491651</v>
       </c>
@@ -19521,7 +19521,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="256" spans="1:14" ht="165" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:14" ht="144" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>491694</v>
       </c>
@@ -19565,7 +19565,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="257" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>491707</v>
       </c>
@@ -19609,7 +19609,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="258" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>491720</v>
       </c>
@@ -19653,7 +19653,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="259" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>491738</v>
       </c>
@@ -19697,7 +19697,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="260" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>491787</v>
       </c>
@@ -19741,7 +19741,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="261" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>491890</v>
       </c>
@@ -19785,7 +19785,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="262" spans="1:14" ht="165" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:14" ht="144" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>491926</v>
       </c>
@@ -19829,7 +19829,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="263" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>492026</v>
       </c>
@@ -19873,7 +19873,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="264" spans="1:14" ht="150" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>492029</v>
       </c>
@@ -19917,7 +19917,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="265" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>492115</v>
       </c>
@@ -19961,7 +19961,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="266" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>492291</v>
       </c>
@@ -19999,7 +19999,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="267" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>492646</v>
       </c>
@@ -20043,7 +20043,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="268" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>492654</v>
       </c>
@@ -20087,7 +20087,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="269" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>492806</v>
       </c>
@@ -20131,7 +20131,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="270" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>492962</v>
       </c>
@@ -20175,7 +20175,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="271" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>493044</v>
       </c>
@@ -20219,7 +20219,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="272" spans="1:14" ht="270" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:14" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>493121</v>
       </c>
@@ -20263,7 +20263,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="273" spans="1:14" ht="180" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>493212</v>
       </c>
@@ -20307,7 +20307,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="274" spans="1:14" ht="330" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:14" ht="288" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>493223</v>
       </c>
@@ -20351,7 +20351,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="275" spans="1:14" ht="180" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:14" ht="144" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>493340</v>
       </c>
@@ -20395,7 +20395,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="276" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>493372</v>
       </c>
@@ -20439,7 +20439,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="277" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>493542</v>
       </c>
@@ -20483,7 +20483,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="278" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>493570</v>
       </c>
@@ -20527,7 +20527,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="279" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>493598</v>
       </c>
@@ -20571,7 +20571,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="280" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>493664</v>
       </c>
@@ -20615,7 +20615,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="281" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>493670</v>
       </c>
@@ -20659,7 +20659,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="282" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>493702</v>
       </c>
@@ -20703,7 +20703,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="283" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>493898</v>
       </c>
@@ -20747,7 +20747,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="284" spans="1:14" ht="345" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:14" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>493920</v>
       </c>
@@ -20791,7 +20791,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="285" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>493983</v>
       </c>
@@ -20835,7 +20835,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="286" spans="1:14" ht="285" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:14" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>494102</v>
       </c>
@@ -20879,7 +20879,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="287" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>494209</v>
       </c>
@@ -20923,7 +20923,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="288" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>494363</v>
       </c>
@@ -20967,7 +20967,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="289" spans="1:14" ht="150" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:14" ht="144" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>494368</v>
       </c>
@@ -21005,7 +21005,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="290" spans="1:14" ht="225" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:14" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>494379</v>
       </c>
@@ -21049,7 +21049,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="291" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>494438</v>
       </c>
@@ -21093,7 +21093,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="292" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>494571</v>
       </c>
@@ -21137,7 +21137,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="293" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>494680</v>
       </c>
@@ -21181,7 +21181,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="294" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>494727</v>
       </c>
@@ -21225,7 +21225,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="295" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>494856</v>
       </c>
@@ -21269,7 +21269,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="296" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>494910</v>
       </c>
@@ -21313,7 +21313,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="297" spans="1:14" ht="225" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:14" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>495152</v>
       </c>
@@ -21357,7 +21357,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="298" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>495320</v>
       </c>
@@ -21401,7 +21401,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="299" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>495442</v>
       </c>
@@ -21445,7 +21445,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="300" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>495504</v>
       </c>
@@ -21489,7 +21489,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="301" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>495595</v>
       </c>
@@ -21533,7 +21533,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="302" spans="1:14" ht="195" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:14" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>495731</v>
       </c>
@@ -21577,7 +21577,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="303" spans="1:14" ht="285" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:14" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>495802</v>
       </c>
@@ -21621,7 +21621,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="304" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>495807</v>
       </c>
@@ -21665,7 +21665,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="305" spans="1:14" ht="165" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:14" ht="144" x14ac:dyDescent="0.3">
       <c r="A305">
         <v>495896</v>
       </c>
@@ -21709,7 +21709,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="306" spans="1:14" ht="285" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:14" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>495942</v>
       </c>
@@ -21747,7 +21747,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="307" spans="1:14" ht="165" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:14" ht="144" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>495969</v>
       </c>
@@ -21791,7 +21791,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="308" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A308">
         <v>496006</v>
       </c>
@@ -21835,7 +21835,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="309" spans="1:14" ht="390" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:14" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>496060</v>
       </c>
@@ -21873,7 +21873,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="310" spans="1:14" ht="180" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>496068</v>
       </c>
@@ -21917,7 +21917,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="311" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>496128</v>
       </c>
@@ -21961,7 +21961,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="312" spans="1:14" ht="225" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:14" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>496154</v>
       </c>
@@ -22005,7 +22005,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="313" spans="1:14" ht="270" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:14" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>496158</v>
       </c>
@@ -22049,7 +22049,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="314" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A314">
         <v>496202</v>
       </c>
@@ -22093,7 +22093,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="315" spans="1:14" ht="165" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:14" ht="144" x14ac:dyDescent="0.3">
       <c r="A315">
         <v>496206</v>
       </c>
@@ -22137,7 +22137,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="316" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A316">
         <v>496274</v>
       </c>
@@ -22181,7 +22181,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="317" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A317">
         <v>496362</v>
       </c>
@@ -22225,7 +22225,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="318" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A318">
         <v>496574</v>
       </c>
@@ -22269,7 +22269,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="319" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A319">
         <v>496577</v>
       </c>
@@ -22313,7 +22313,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="320" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A320">
         <v>496586</v>
       </c>
@@ -22357,7 +22357,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="321" spans="1:14" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:14" ht="360" x14ac:dyDescent="0.3">
       <c r="A321">
         <v>496733</v>
       </c>
@@ -22401,7 +22401,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="322" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A322">
         <v>496772</v>
       </c>

</xml_diff>